<commit_message>
Alerts v2.1.2 fixes 9.27.23
</commit_message>
<xml_diff>
--- a/workload/bicep/brownfield/alerts/references/alerts.xlsx
+++ b/workload/bicep/brownfield/alerts/references/alerts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\avdaccelerator\workload\bicep\brownfield\alerts\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F201D244-014A-4415-B2EF-C1D75F1C67EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8585E4B-E46A-44A6-932C-2628D72D7AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1747E9F3-8C51-4656-9796-47111650C799}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="113">
   <si>
     <t>Alert Name</t>
   </si>
@@ -179,12 +179,6 @@
     <t>Check Azure service availability.  If there is an outage contact Azure Support</t>
   </si>
   <si>
-    <t>Potential performance issues for users on the same host due to critically low memory.</t>
-  </si>
-  <si>
-    <t>Potential performance issues for users on the same host due to moderately low memory.</t>
-  </si>
-  <si>
     <t>Investigate session host memory usage per user and/or memory requirements and adjust if/as needed.  Check user active vs. disconnected status.</t>
   </si>
   <si>
@@ -362,18 +356,6 @@
     <t>There are lots of variables between the end uers and AVD VMs. If this is frequent for the user, determine if their Internet connection is slow or latency is over 150 ms.</t>
   </si>
   <si>
-    <t>AVD-VM-Missing Critical Update(s)</t>
-  </si>
-  <si>
-    <t>1 day</t>
-  </si>
-  <si>
-    <t>The VM is missing approved Critical Updates</t>
-  </si>
-  <si>
-    <t>Ensure patching is working as expected and update the VM as soon as possible.</t>
-  </si>
-  <si>
     <t>AVD-VM-FSLogix Profile Disk Attached to another VM</t>
   </si>
   <si>
@@ -383,10 +365,16 @@
     <t>This indicates that a user attempted to load their profile disk but it was in use or possibly mapped to another VM. Ensure the user is not connected to another host pool or remote app with the same profile.</t>
   </si>
   <si>
-    <t>Potential performance issues for users on the same host due to critically limited CPU (Avarage over 5 mins.)</t>
-  </si>
-  <si>
-    <t>Potential performance issues for users on the same host due to moderately limited CPU (Avarage over 5 mins.)</t>
+    <t>Potential performance issues for users on the same host due to critically limited CPU (Avarage over 15 mins.)</t>
+  </si>
+  <si>
+    <t>Potential performance issues for users on the same host due to moderately limited CPU (Avarage over 15 mins.)</t>
+  </si>
+  <si>
+    <t>Potential performance issues for users on the same host due to critically low memory. (avg over 15min)</t>
+  </si>
+  <si>
+    <t>Potential performance issues for users on the same host due to moderately low memory. (avg over 15min)</t>
   </si>
 </sst>
 </file>
@@ -651,18 +639,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -971,7 +959,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -979,24 +967,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D25CA4-DB62-4CFC-AE65-12A371E961DC}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="73.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" customWidth="1"/>
-    <col min="4" max="5" width="22.7265625" customWidth="1"/>
-    <col min="6" max="6" width="42.6328125" customWidth="1"/>
-    <col min="7" max="7" width="44.90625" customWidth="1"/>
+    <col min="2" max="2" width="73.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.73046875" customWidth="1"/>
+    <col min="4" max="5" width="22.73046875" customWidth="1"/>
+    <col min="6" max="6" width="42.59765625" customWidth="1"/>
+    <col min="7" max="7" width="44.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1004,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1036,10 +1024,10 @@
         <v>38</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="33"/>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1057,13 +1045,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="33"/>
       <c r="B4" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="11">
         <v>1</v>
@@ -1075,13 +1063,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="33"/>
       <c r="B5" s="7" t="s">
         <v>11</v>
@@ -1099,11 +1087,11 @@
         <v>36</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="35"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="34"/>
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1120,10 +1108,10 @@
         <v>37</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1132,8 +1120,8 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1149,13 +1137,13 @@
         <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="33"/>
       <c r="B9" s="15" t="s">
         <v>17</v>
@@ -1170,13 +1158,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="33"/>
       <c r="B10" s="10" t="s">
         <v>18</v>
@@ -1191,13 +1179,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="33"/>
       <c r="B11" s="15" t="s">
         <v>19</v>
@@ -1212,16 +1200,16 @@
         <v>10</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="33"/>
       <c r="B12" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="11">
         <v>2</v>
@@ -1236,13 +1224,13 @@
         <v>42</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="33"/>
       <c r="B13" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="16">
         <v>1</v>
@@ -1257,13 +1245,13 @@
         <v>42</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="33"/>
       <c r="B14" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="11">
         <v>1</v>
@@ -1278,13 +1266,13 @@
         <v>42</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="33"/>
       <c r="B15" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="16">
         <v>2</v>
@@ -1299,10 +1287,10 @@
         <v>42</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="33"/>
       <c r="B16" s="10" t="s">
         <v>20</v>
@@ -1323,8 +1311,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="34"/>
       <c r="B17" s="15" t="s">
         <v>39</v>
       </c>
@@ -1344,7 +1332,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1353,8 +1341,8 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="32" t="s">
+    <row r="19" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="37" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1370,13 +1358,13 @@
         <v>7</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="33"/>
       <c r="B20" s="18" t="s">
         <v>23</v>
@@ -1391,16 +1379,16 @@
         <v>7</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="33"/>
       <c r="B21" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="11">
         <v>1</v>
@@ -1412,16 +1400,16 @@
         <v>7</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="33"/>
       <c r="B22" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
@@ -1433,16 +1421,16 @@
         <v>7</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="33"/>
       <c r="B23" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" s="11">
         <v>1</v>
@@ -1454,16 +1442,16 @@
         <v>7</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="33"/>
       <c r="B24" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="19">
         <v>1</v>
@@ -1475,16 +1463,16 @@
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="33"/>
       <c r="B25" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="11">
         <v>1</v>
@@ -1496,16 +1484,16 @@
         <v>7</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="33"/>
       <c r="B26" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" s="19">
         <v>1</v>
@@ -1517,16 +1505,16 @@
         <v>7</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="78.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="78.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="33"/>
       <c r="B27" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
@@ -1538,13 +1526,13 @@
         <v>7</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="33"/>
       <c r="B28" s="18" t="s">
         <v>24</v>
@@ -1559,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="33"/>
       <c r="B29" s="4" t="s">
         <v>25</v>
@@ -1580,13 +1568,13 @@
         <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="33"/>
       <c r="B30" s="18" t="s">
         <v>26</v>
@@ -1601,13 +1589,13 @@
         <v>7</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="33"/>
       <c r="B31" s="4" t="s">
         <v>27</v>
@@ -1622,13 +1610,13 @@
         <v>13</v>
       </c>
       <c r="F31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:7" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="33"/>
       <c r="B32" s="18" t="s">
         <v>28</v>
@@ -1643,16 +1631,16 @@
         <v>13</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="33"/>
       <c r="B33" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="5">
         <v>1</v>
@@ -1664,16 +1652,16 @@
         <v>7</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="33"/>
       <c r="B34" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C34" s="19">
         <v>2</v>
@@ -1685,16 +1673,16 @@
         <v>7</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="33"/>
       <c r="B35" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -1706,179 +1694,158 @@
         <v>7</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="33"/>
       <c r="B36" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C36" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="33"/>
-      <c r="B37" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="5">
-        <v>3</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="4" t="s">
+    </row>
+    <row r="37" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A38" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="5">
+        <v>4</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="33"/>
+      <c r="B39" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="22">
+        <v>4</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="33"/>
+      <c r="B40" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="11">
         <v>4</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="33"/>
-      <c r="B40" s="24" t="s">
+      <c r="D40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="34"/>
+      <c r="B41" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C41" s="22">
         <v>4</v>
       </c>
-      <c r="D40" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="33"/>
-      <c r="B41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="11">
-        <v>4</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="35"/>
-      <c r="B42" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="22">
-        <v>4</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D41" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="27"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="27"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="31" t="s">
+    <row r="46" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="30" t="s">
         <v>94</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A8:A17"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A19:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A19:A36"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>